<commit_message>
Addition of catch in reset password and order date object modified
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/SignUp.xlsx
+++ b/binaries/FCfiles/SignUp.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="368">
   <si>
     <t>shipmentType</t>
   </si>
@@ -1128,6 +1128,9 @@
   </si>
   <si>
     <t>SeleniumcnpG@mailinator.com</t>
+  </si>
+  <si>
+    <t>Automation9587!</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1154,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="506">
+  <fills count="508">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3678,8 +3681,18 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="502">
+  <borders count="504">
     <border>
       <left/>
       <right/>
@@ -5510,6 +5523,13 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -5518,7 +5538,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="269">
+  <cellXfs count="270">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -5787,7 +5807,8 @@
     <xf applyBorder="true" applyFill="true" borderId="495" fillId="499" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="497" fillId="501" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="499" fillId="503" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="505" borderId="501" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="501" fillId="505" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="507" borderId="503" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -6297,8 +6318,8 @@
       <c r="E7" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="F7" s="262" t="s">
-        <v>360</v>
+      <c r="F7" s="269" t="s">
+        <v>367</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Updation of log jars
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/SignUp.xlsx
+++ b/binaries/FCfiles/SignUp.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="405">
   <si>
     <t>shipmentType</t>
   </si>
@@ -1239,6 +1239,9 @@
   </si>
   <si>
     <t>Automation4435!</t>
+  </si>
+  <si>
+    <t>SeleniummuDA@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -1262,7 +1265,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="580">
+  <fills count="582">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4159,8 +4162,18 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="576">
+  <borders count="578">
     <border>
       <left/>
       <right/>
@@ -6250,6 +6263,13 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -6258,7 +6278,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="306">
+  <cellXfs count="307">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -6564,7 +6584,8 @@
     <xf applyBorder="true" applyFill="true" borderId="569" fillId="573" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="571" fillId="575" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="573" fillId="577" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="579" borderId="575" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="575" fillId="579" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="581" borderId="577" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -6911,8 +6932,8 @@
       <c r="D2" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="299" t="s">
-        <v>397</v>
+      <c r="E2" s="306" t="s">
+        <v>404</v>
       </c>
       <c r="F2" t="s">
         <v>40</v>

</xml_diff>